<commit_message>
The columns in excel will now be headered with the corresponding edf file name.
</commit_message>
<xml_diff>
--- a/PutData.xlsx
+++ b/PutData.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,7 +18,7 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -425,17 +425,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>GHI</t>
         </is>
       </c>
     </row>
@@ -639,17 +639,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>GHI</t>
         </is>
       </c>
     </row>
@@ -853,17 +853,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>GHI</t>
         </is>
       </c>
     </row>
@@ -1067,17 +1067,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>ABC</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>DEF</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>GHI</t>
         </is>
       </c>
     </row>

</xml_diff>